<commit_message>
Renamed bop architecture 22copy to 10. Created dictionary to analyse the different architectures 10, 21,22 and 23
</commit_message>
<xml_diff>
--- a/04_thermal/03_python/results.xlsx
+++ b/04_thermal/03_python/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,50 +436,55 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Vdot_1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Vdot el. Comp. in [l/s]</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Vdot Intercooler in [l/s]</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>LV DCDC T_in in [°C]</t>
-        </is>
-      </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>HV DCDC T_in in [°C]</t>
+          <t>LV DCDC T_in</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Inverter T_in in [°C]</t>
+          <t>HV DCDC T_in</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>HPDU T_in in [°C]</t>
+          <t>Inverter T_in</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Compressor T_in in [°C]</t>
+          <t>HPDU T_in</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Intercooler T_in in [°C]</t>
+          <t>Compressor T_in</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>BoP T_out in [°C]</t>
+          <t>Intercooler T_in</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>BoP T_out</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>P_out in [bar]</t>
         </is>
@@ -490,34 +495,37 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.2031515571918942</v>
+        <v>0.25</v>
       </c>
       <c r="C2" t="n">
-        <v>0.04684844280810583</v>
+        <v>0.08059539500474169</v>
       </c>
       <c r="D2" t="n">
+        <v>0.1694046049952583</v>
+      </c>
+      <c r="E2" t="n">
         <v>312.1704476099254</v>
       </c>
-      <c r="E2" t="n">
-        <v>317.70676633787</v>
-      </c>
       <c r="F2" t="n">
-        <v>314.9938973253738</v>
+        <v>312.3507121569987</v>
       </c>
       <c r="G2" t="n">
-        <v>312.8222345175304</v>
+        <v>313.4332218419817</v>
       </c>
       <c r="H2" t="n">
-        <v>321.1773747330067</v>
+        <v>312.1704476099254</v>
       </c>
       <c r="I2" t="n">
-        <v>312.1704476099254</v>
+        <v>315.0110017603065</v>
       </c>
       <c r="J2" t="n">
+        <v>313.3119395659741</v>
+      </c>
+      <c r="K2" t="n">
         <v>324.836433382633</v>
       </c>
-      <c r="K2" t="n">
-        <v>0.8540077657044012</v>
+      <c r="L2" t="n">
+        <v>0.7506248225323764</v>
       </c>
     </row>
     <row r="3">
@@ -525,34 +533,37 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2703526857231149</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="C3" t="n">
-        <v>0.06298031427688508</v>
+        <v>0.1059956085962485</v>
       </c>
       <c r="D3" t="n">
-        <v>314.9177038178763</v>
+        <v>0.2273373914037499</v>
       </c>
       <c r="E3" t="n">
-        <v>319.0339059454114</v>
+        <v>314.9177038178762</v>
       </c>
       <c r="F3" t="n">
-        <v>317.0165900071119</v>
+        <v>315.0519199006713</v>
       </c>
       <c r="G3" t="n">
-        <v>315.4021559487556</v>
+        <v>315.877150067895</v>
       </c>
       <c r="H3" t="n">
-        <v>321.6152681676467</v>
+        <v>314.9177038178762</v>
       </c>
       <c r="I3" t="n">
-        <v>314.9177038178763</v>
+        <v>317.0761544598553</v>
       </c>
       <c r="J3" t="n">
-        <v>324.4148216346758</v>
+        <v>315.7676611761784</v>
       </c>
       <c r="K3" t="n">
-        <v>0.7628292411861662</v>
+        <v>324.4148216347054</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.5915138621357861</v>
       </c>
     </row>
     <row r="4">
@@ -560,34 +571,37 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.3375211262450013</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="C4" t="n">
-        <v>0.07914587375499872</v>
+        <v>0.1313263722084737</v>
       </c>
       <c r="D4" t="n">
+        <v>0.2853406277915264</v>
+      </c>
+      <c r="E4" t="n">
         <v>316.5650743986903</v>
       </c>
-      <c r="E4" t="n">
-        <v>319.8397726938424</v>
-      </c>
       <c r="F4" t="n">
-        <v>318.2347508871371</v>
+        <v>316.6719656471541</v>
       </c>
       <c r="G4" t="n">
-        <v>316.9504326975884</v>
+        <v>317.3391841463729</v>
       </c>
       <c r="H4" t="n">
-        <v>321.8937813060626</v>
+        <v>316.5650743986903</v>
       </c>
       <c r="I4" t="n">
-        <v>316.5650743986903</v>
+        <v>318.3066606681732</v>
       </c>
       <c r="J4" t="n">
+        <v>317.2420121325483</v>
+      </c>
+      <c r="K4" t="n">
         <v>324.1618541532335</v>
       </c>
-      <c r="K4" t="n">
-        <v>0.6503970390654911</v>
+      <c r="L4" t="n">
+        <v>0.394463876324013</v>
       </c>
     </row>
     <row r="5">
@@ -595,34 +609,37 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.4046702673523267</v>
+        <v>0.5</v>
       </c>
       <c r="C5" t="n">
-        <v>0.09532973264767332</v>
+        <v>0.1566188491071225</v>
       </c>
       <c r="D5" t="n">
+        <v>0.3433811508928775</v>
+      </c>
+      <c r="E5" t="n">
         <v>317.6629731430928</v>
       </c>
-      <c r="E5" t="n">
-        <v>320.3813808876369</v>
-      </c>
       <c r="F5" t="n">
-        <v>319.048958290813</v>
+        <v>317.7517777873888</v>
       </c>
       <c r="G5" t="n">
-        <v>317.9828440863042</v>
+        <v>318.3119444875464</v>
       </c>
       <c r="H5" t="n">
-        <v>322.0866340269861</v>
+        <v>317.6629731430928</v>
       </c>
       <c r="I5" t="n">
-        <v>317.6629731430928</v>
+        <v>319.1230630964595</v>
       </c>
       <c r="J5" t="n">
-        <v>323.9932120428593</v>
+        <v>318.2253790890475</v>
       </c>
       <c r="K5" t="n">
-        <v>0.5167139912075003</v>
+        <v>323.9932120428591</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.1594804941517815</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Input Architectures Bop adapted to be further anlysed
</commit_message>
<xml_diff>
--- a/04_thermal/03_python/results.xlsx
+++ b/04_thermal/03_python/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,37 +495,37 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.25</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="C2" t="n">
-        <v>0.08059539500474169</v>
+        <v>0.08058607483302643</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1694046049952583</v>
+        <v>0.08608092516697356</v>
       </c>
       <c r="E2" t="n">
-        <v>312.1704476099254</v>
+        <v>306.66746069682</v>
       </c>
       <c r="F2" t="n">
-        <v>312.3507121569987</v>
+        <v>307.0230317067672</v>
       </c>
       <c r="G2" t="n">
-        <v>313.4332218419817</v>
+        <v>307.9332303460307</v>
       </c>
       <c r="H2" t="n">
-        <v>312.1704476099254</v>
+        <v>306.66746069682</v>
       </c>
       <c r="I2" t="n">
-        <v>315.0110017603065</v>
+        <v>308.9183798995069</v>
       </c>
       <c r="J2" t="n">
-        <v>313.3119395659741</v>
+        <v>309.8179771970586</v>
       </c>
       <c r="K2" t="n">
-        <v>324.836433382633</v>
+        <v>325.6796778876795</v>
       </c>
       <c r="L2" t="n">
-        <v>0.7506248225323764</v>
+        <v>0.7790629194950628</v>
       </c>
     </row>
     <row r="3">
@@ -533,37 +533,37 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.2166666666666667</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1059956085962485</v>
+        <v>0.1055058401668167</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2273373914037499</v>
+        <v>0.1111611598331833</v>
       </c>
       <c r="E3" t="n">
-        <v>314.9177038178762</v>
+        <v>310.4785776821093</v>
       </c>
       <c r="F3" t="n">
-        <v>315.0519199006713</v>
+        <v>310.7534595537888</v>
       </c>
       <c r="G3" t="n">
-        <v>315.877150067895</v>
+        <v>311.4438362575175</v>
       </c>
       <c r="H3" t="n">
-        <v>314.9177038178762</v>
+        <v>310.4785776821093</v>
       </c>
       <c r="I3" t="n">
-        <v>317.0761544598553</v>
+        <v>312.2190145692873</v>
       </c>
       <c r="J3" t="n">
-        <v>315.7676611761784</v>
+        <v>312.8986012346134</v>
       </c>
       <c r="K3" t="n">
-        <v>324.4148216347054</v>
+        <v>325.0958879058764</v>
       </c>
       <c r="L3" t="n">
-        <v>0.5915138621357861</v>
+        <v>0.6527110314384649</v>
       </c>
     </row>
     <row r="4">
@@ -571,37 +571,37 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.2666666666666667</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1313263722084737</v>
+        <v>0.1304563450453853</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2853406277915264</v>
+        <v>0.1362106549546147</v>
       </c>
       <c r="E4" t="n">
-        <v>316.5650743986903</v>
+        <v>312.8574984796292</v>
       </c>
       <c r="F4" t="n">
-        <v>316.6719656471541</v>
+        <v>313.0816395885642</v>
       </c>
       <c r="G4" t="n">
-        <v>317.3391841463729</v>
+        <v>313.6375222630601</v>
       </c>
       <c r="H4" t="n">
-        <v>316.5650743986903</v>
+        <v>312.8574984796292</v>
       </c>
       <c r="I4" t="n">
-        <v>318.3066606681732</v>
+        <v>314.2767951394444</v>
       </c>
       <c r="J4" t="n">
-        <v>317.2420121325483</v>
+        <v>314.8223685259341</v>
       </c>
       <c r="K4" t="n">
-        <v>324.1618541532335</v>
+        <v>324.7310275843784</v>
       </c>
       <c r="L4" t="n">
-        <v>0.394463876324013</v>
+        <v>0.4986528269812863</v>
       </c>
     </row>
     <row r="5">
@@ -609,37 +609,75 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.5</v>
+        <v>0.3166666666666667</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1566188491071225</v>
+        <v>0.1554241421537281</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3433811508928775</v>
+        <v>0.1612428578462719</v>
       </c>
       <c r="E5" t="n">
-        <v>317.6629731430928</v>
+        <v>314.4840917792948</v>
       </c>
       <c r="F5" t="n">
-        <v>317.7517777873888</v>
+        <v>314.6733446756259</v>
       </c>
       <c r="G5" t="n">
-        <v>318.3119444875464</v>
+        <v>315.1385109103733</v>
       </c>
       <c r="H5" t="n">
-        <v>317.6629731430928</v>
+        <v>314.4840917792948</v>
       </c>
       <c r="I5" t="n">
-        <v>319.1230630964595</v>
+        <v>315.6825332862946</v>
       </c>
       <c r="J5" t="n">
-        <v>318.2253790890475</v>
+        <v>316.1380456860362</v>
       </c>
       <c r="K5" t="n">
-        <v>323.9932120428591</v>
+        <v>324.4813890718348</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1594804941517815</v>
+        <v>0.316888550462615</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.3666666666666666</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.1804026295365585</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.1862643704634415</v>
+      </c>
+      <c r="E6" t="n">
+        <v>315.6665988481321</v>
+      </c>
+      <c r="F6" t="n">
+        <v>315.8303792725541</v>
+      </c>
+      <c r="G6" t="n">
+        <v>316.2302458203413</v>
+      </c>
+      <c r="H6" t="n">
+        <v>315.6665988481321</v>
+      </c>
+      <c r="I6" t="n">
+        <v>316.7037701672701</v>
+      </c>
+      <c r="J6" t="n">
+        <v>317.0946492976096</v>
+      </c>
+      <c r="K6" t="n">
+        <v>324.299834870174</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.1074183015888076</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed plotting a bit. Absolute Pressure to Pressure difference. Renamed arch 34 to 41
</commit_message>
<xml_diff>
--- a/04_thermal/03_python/results.xlsx
+++ b/04_thermal/03_python/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,37 +495,37 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.25</v>
       </c>
       <c r="C2" t="n">
-        <v>0.08058607483302643</v>
+        <v>0.04684844280810583</v>
       </c>
       <c r="D2" t="n">
-        <v>0.08608092516697356</v>
+        <v>0.2031515571918942</v>
       </c>
       <c r="E2" t="n">
-        <v>306.66746069682</v>
+        <v>312.1704476099254</v>
       </c>
       <c r="F2" t="n">
-        <v>307.0230317067672</v>
+        <v>317.70676633787</v>
       </c>
       <c r="G2" t="n">
-        <v>307.9332303460307</v>
+        <v>314.9938973253738</v>
       </c>
       <c r="H2" t="n">
-        <v>306.66746069682</v>
+        <v>312.8222345175304</v>
       </c>
       <c r="I2" t="n">
-        <v>308.9183798995069</v>
+        <v>321.1773747330067</v>
       </c>
       <c r="J2" t="n">
-        <v>309.8179771970586</v>
+        <v>312.1704476099254</v>
       </c>
       <c r="K2" t="n">
-        <v>325.6796778876795</v>
+        <v>324.836433382633</v>
       </c>
       <c r="L2" t="n">
-        <v>0.7790629194950628</v>
+        <v>0.1459922342955988</v>
       </c>
     </row>
     <row r="3">
@@ -533,37 +533,37 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2166666666666667</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1055058401668167</v>
+        <v>0.06298031427688508</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1111611598331833</v>
+        <v>0.2703526857231149</v>
       </c>
       <c r="E3" t="n">
-        <v>310.4785776821093</v>
+        <v>314.9177038178763</v>
       </c>
       <c r="F3" t="n">
-        <v>310.7534595537888</v>
+        <v>319.0339059454114</v>
       </c>
       <c r="G3" t="n">
-        <v>311.4438362575175</v>
+        <v>317.0165900071119</v>
       </c>
       <c r="H3" t="n">
-        <v>310.4785776821093</v>
+        <v>315.4021559487556</v>
       </c>
       <c r="I3" t="n">
-        <v>312.2190145692873</v>
+        <v>321.6152681676467</v>
       </c>
       <c r="J3" t="n">
-        <v>312.8986012346134</v>
+        <v>314.9177038178763</v>
       </c>
       <c r="K3" t="n">
-        <v>325.0958879058764</v>
+        <v>324.4148216346758</v>
       </c>
       <c r="L3" t="n">
-        <v>0.6527110314384649</v>
+        <v>0.2371707588138338</v>
       </c>
     </row>
     <row r="4">
@@ -571,37 +571,37 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.2666666666666667</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1304563450453853</v>
+        <v>0.07914587375499872</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1362106549546147</v>
+        <v>0.3375211262450013</v>
       </c>
       <c r="E4" t="n">
-        <v>312.8574984796292</v>
+        <v>316.5650743986903</v>
       </c>
       <c r="F4" t="n">
-        <v>313.0816395885642</v>
+        <v>319.8397726938424</v>
       </c>
       <c r="G4" t="n">
-        <v>313.6375222630601</v>
+        <v>318.2347508871371</v>
       </c>
       <c r="H4" t="n">
-        <v>312.8574984796292</v>
+        <v>316.9504326975884</v>
       </c>
       <c r="I4" t="n">
-        <v>314.2767951394444</v>
+        <v>321.8937813060626</v>
       </c>
       <c r="J4" t="n">
-        <v>314.8223685259341</v>
+        <v>316.5650743986903</v>
       </c>
       <c r="K4" t="n">
-        <v>324.7310275843784</v>
+        <v>324.1618541532335</v>
       </c>
       <c r="L4" t="n">
-        <v>0.4986528269812863</v>
+        <v>0.3496029609345089</v>
       </c>
     </row>
     <row r="5">
@@ -609,75 +609,37 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.3166666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1554241421537281</v>
+        <v>0.09532973264767332</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1612428578462719</v>
+        <v>0.4046702673523267</v>
       </c>
       <c r="E5" t="n">
-        <v>314.4840917792948</v>
+        <v>317.6629731430928</v>
       </c>
       <c r="F5" t="n">
-        <v>314.6733446756259</v>
+        <v>320.3813808876369</v>
       </c>
       <c r="G5" t="n">
-        <v>315.1385109103733</v>
+        <v>319.048958290813</v>
       </c>
       <c r="H5" t="n">
-        <v>314.4840917792948</v>
+        <v>317.9828440863042</v>
       </c>
       <c r="I5" t="n">
-        <v>315.6825332862946</v>
+        <v>322.0866340269861</v>
       </c>
       <c r="J5" t="n">
-        <v>316.1380456860362</v>
+        <v>317.6629731430928</v>
       </c>
       <c r="K5" t="n">
-        <v>324.4813890718348</v>
+        <v>323.9932120428593</v>
       </c>
       <c r="L5" t="n">
-        <v>0.316888550462615</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.3666666666666666</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.1804026295365585</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.1862643704634415</v>
-      </c>
-      <c r="E6" t="n">
-        <v>315.6665988481321</v>
-      </c>
-      <c r="F6" t="n">
-        <v>315.8303792725541</v>
-      </c>
-      <c r="G6" t="n">
-        <v>316.2302458203413</v>
-      </c>
-      <c r="H6" t="n">
-        <v>315.6665988481321</v>
-      </c>
-      <c r="I6" t="n">
-        <v>316.7037701672701</v>
-      </c>
-      <c r="J6" t="n">
-        <v>317.0946492976096</v>
-      </c>
-      <c r="K6" t="n">
-        <v>324.299834870174</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.1074183015888076</v>
+        <v>0.4832860087924997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New BoP pressure drop, equal to archticture 21.
</commit_message>
<xml_diff>
--- a/04_thermal/03_python/results.xlsx
+++ b/04_thermal/03_python/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,7 +486,7 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>P_out in [bar]</t>
+          <t>bop pressure drop in [bar]</t>
         </is>
       </c>
     </row>
@@ -495,37 +495,37 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.25</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="C2" t="n">
-        <v>0.04684844280810583</v>
+        <v>0.03078718242887758</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2031515571918942</v>
+        <v>0.1358798175711224</v>
       </c>
       <c r="E2" t="n">
-        <v>312.1704476099254</v>
+        <v>306.6674606968199</v>
       </c>
       <c r="F2" t="n">
-        <v>317.70676633787</v>
+        <v>315.1035309651432</v>
       </c>
       <c r="G2" t="n">
-        <v>314.9938973253738</v>
+        <v>310.9716196524392</v>
       </c>
       <c r="H2" t="n">
-        <v>312.8222345175304</v>
+        <v>307.6614797046352</v>
       </c>
       <c r="I2" t="n">
-        <v>321.1773747330067</v>
+        <v>320.3861989161594</v>
       </c>
       <c r="J2" t="n">
-        <v>312.1704476099254</v>
+        <v>306.6674606968199</v>
       </c>
       <c r="K2" t="n">
-        <v>324.836433382633</v>
+        <v>325.6796778876807</v>
       </c>
       <c r="L2" t="n">
-        <v>0.1459922342955988</v>
+        <v>0.07606633230618498</v>
       </c>
     </row>
     <row r="3">
@@ -533,37 +533,37 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.2</v>
       </c>
       <c r="C3" t="n">
-        <v>0.06298031427688508</v>
+        <v>0.03719881950877927</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2703526857231149</v>
+        <v>0.1628011804912188</v>
       </c>
       <c r="E3" t="n">
-        <v>314.9177038178763</v>
+        <v>309.4205584734395</v>
       </c>
       <c r="F3" t="n">
-        <v>319.0339059454114</v>
+        <v>316.3973690341517</v>
       </c>
       <c r="G3" t="n">
-        <v>317.0165900071119</v>
+        <v>312.9793391096121</v>
       </c>
       <c r="H3" t="n">
-        <v>315.4021559487556</v>
+        <v>310.2422489515129</v>
       </c>
       <c r="I3" t="n">
-        <v>321.6152681676467</v>
+        <v>320.7688472191118</v>
       </c>
       <c r="J3" t="n">
-        <v>314.9177038178763</v>
+        <v>309.4205584734395</v>
       </c>
       <c r="K3" t="n">
-        <v>324.4148216346758</v>
+        <v>325.2580534501679</v>
       </c>
       <c r="L3" t="n">
-        <v>0.2371707588138338</v>
+        <v>0.1014861590692906</v>
       </c>
     </row>
     <row r="4">
@@ -571,37 +571,37 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.25</v>
       </c>
       <c r="C4" t="n">
-        <v>0.07914587375499872</v>
+        <v>0.04684844280810583</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3375211262450013</v>
+        <v>0.2031515571918942</v>
       </c>
       <c r="E4" t="n">
-        <v>316.5650743986903</v>
+        <v>312.1704476099254</v>
       </c>
       <c r="F4" t="n">
-        <v>319.8397726938424</v>
+        <v>317.70676633787</v>
       </c>
       <c r="G4" t="n">
-        <v>318.2347508871371</v>
+        <v>314.9938973253738</v>
       </c>
       <c r="H4" t="n">
-        <v>316.9504326975884</v>
+        <v>312.8222345175304</v>
       </c>
       <c r="I4" t="n">
-        <v>321.8937813060626</v>
+        <v>321.1773747330067</v>
       </c>
       <c r="J4" t="n">
-        <v>316.5650743986903</v>
+        <v>312.1704476099254</v>
       </c>
       <c r="K4" t="n">
-        <v>324.1618541532335</v>
+        <v>324.836433382633</v>
       </c>
       <c r="L4" t="n">
-        <v>0.3496029609345089</v>
+        <v>0.1459922342955988</v>
       </c>
     </row>
     <row r="5">
@@ -609,36 +609,226 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
+        <v>0.2833333333333333</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.05329556577176932</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.2300374342282307</v>
+      </c>
+      <c r="E5" t="n">
+        <v>313.4635556567899</v>
+      </c>
+      <c r="F5" t="n">
+        <v>318.3289404428087</v>
+      </c>
+      <c r="G5" t="n">
+        <v>315.9446451588739</v>
+      </c>
+      <c r="H5" t="n">
+        <v>314.036267093806</v>
+      </c>
+      <c r="I5" t="n">
+        <v>321.3795479015832</v>
+      </c>
+      <c r="J5" t="n">
+        <v>313.4635556567899</v>
+      </c>
+      <c r="K5" t="n">
+        <v>324.6380282756148</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.1799131506506343</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.06298031427688508</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.2703526857231149</v>
+      </c>
+      <c r="E6" t="n">
+        <v>314.9177038178763</v>
+      </c>
+      <c r="F6" t="n">
+        <v>319.0339059454114</v>
+      </c>
+      <c r="G6" t="n">
+        <v>317.0165900071119</v>
+      </c>
+      <c r="H6" t="n">
+        <v>315.4021559487556</v>
+      </c>
+      <c r="I6" t="n">
+        <v>321.6152681676467</v>
+      </c>
+      <c r="J6" t="n">
+        <v>314.9177038178763</v>
+      </c>
+      <c r="K6" t="n">
+        <v>324.4148216346758</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.2371707588138338</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.3666666666666666</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.06944369957187221</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.2972233004281278</v>
+      </c>
+      <c r="E7" t="n">
+        <v>315.6665988481321</v>
+      </c>
+      <c r="F7" t="n">
+        <v>319.3992706452299</v>
+      </c>
+      <c r="G7" t="n">
+        <v>317.5698539854616</v>
+      </c>
+      <c r="H7" t="n">
+        <v>316.1058821987543</v>
+      </c>
+      <c r="I7" t="n">
+        <v>321.7403163081778</v>
+      </c>
+      <c r="J7" t="n">
+        <v>315.6665988481321</v>
+      </c>
+      <c r="K7" t="n">
+        <v>324.299834870174</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.2795938541944102</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.4166666666666667</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.07914587375499872</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.3375211262450013</v>
+      </c>
+      <c r="E8" t="n">
+        <v>316.5650743986903</v>
+      </c>
+      <c r="F8" t="n">
+        <v>319.8397726938424</v>
+      </c>
+      <c r="G8" t="n">
+        <v>318.2347508871371</v>
+      </c>
+      <c r="H8" t="n">
+        <v>316.9504326975884</v>
+      </c>
+      <c r="I8" t="n">
+        <v>321.8937813060626</v>
+      </c>
+      <c r="J8" t="n">
+        <v>316.5650743986903</v>
+      </c>
+      <c r="K8" t="n">
+        <v>324.1618541532335</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.3496029609345089</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.08561766907149518</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.3643823309285048</v>
+      </c>
+      <c r="E9" t="n">
+        <v>317.0530562460292</v>
+      </c>
+      <c r="F9" t="n">
+        <v>320.0800385932849</v>
+      </c>
+      <c r="G9" t="n">
+        <v>318.5964010967026</v>
+      </c>
+      <c r="H9" t="n">
+        <v>317.4092512500918</v>
+      </c>
+      <c r="I9" t="n">
+        <v>321.9787589386128</v>
+      </c>
+      <c r="J9" t="n">
+        <v>317.0530562460292</v>
+      </c>
+      <c r="K9" t="n">
+        <v>324.0869024983483</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.4005256201793522</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
         <v>0.5</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C10" t="n">
         <v>0.09532973264767332</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D10" t="n">
         <v>0.4046702673523267</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E10" t="n">
         <v>317.6629731430928</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F10" t="n">
         <v>320.3813808876369</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G10" t="n">
         <v>319.048958290813</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H10" t="n">
         <v>317.9828440863042</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I10" t="n">
         <v>322.0866340269861</v>
       </c>
-      <c r="J5" t="n">
+      <c r="J10" t="n">
         <v>317.6629731430928</v>
       </c>
-      <c r="K5" t="n">
+      <c r="K10" t="n">
         <v>323.9932120428593</v>
       </c>
-      <c r="L5" t="n">
+      <c r="L10" t="n">
         <v>0.4832860087924997</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new folder structure -> improved overview
</commit_message>
<xml_diff>
--- a/04_thermal/03_python/results.xlsx
+++ b/04_thermal/03_python/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:AX3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,57 +436,247 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Vdot_1</t>
+          <t>Arch01_pump_vdot</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Vdot el. Comp. in [l/s]</t>
+          <t>Arch01_pump_delta_p</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Vdot Intercooler in [l/s]</t>
+          <t>Arch01_radiator_vdot</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>LV DCDC T_in</t>
+          <t>Arch01_perc_recirc</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>HV DCDC T_in</t>
+          <t>Arch01_radiator_t_in</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Inverter T_in</t>
+          <t>Arch01_pump2_vdot</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>HPDU T_in</t>
+          <t>Arch01_pump2_delta_p</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Compressor T_in</t>
+          <t>Arch03a_pump_vdot</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Intercooler T_in</t>
+          <t>Arch03a_pump_delta_p</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>BoP T_out</t>
+          <t>Arch03a_radiator_vdot</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>bop pressure drop in [bar]</t>
+          <t>Arch03a_perc_recirc</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Arch03a_radiator_t_in</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Arch03a_pump2_vdot</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Arch03a_pump2_delta_p</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Arch03b_pump_vdot</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Arch03b_pump_delta_p</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Arch03b_radiator_vdot</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Arch03b_perc_recirc</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Arch03b_radiator_t_in</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Arch03b_pump2_vdot</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Arch03b_pump2_delta_p</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Arch04_pump_vdot</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Arch04_pump_delta_p</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Arch04_radiator_vdot</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Arch04_perc_recirc</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Arch04_radiator_t_in</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Arch04_pump2_vdot</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Arch04_pump2_delta_p</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Arch05_pump_vdot</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Arch05_pump_delta_p</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Arch05_radiator_vdot</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Arch05_perc_recirc</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Arch05_radiator_t_in</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Arch05_pump2_vdot</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Arch05_pump2_delta_p</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Arch06_pump_vdot</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Arch06_pump_delta_p</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>Arch06_radiator_vdot</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Arch06_perc_recirc</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Arch06_radiator_t_in</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>Arch06_pump2_vdot</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Arch06_pump2_delta_p</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>Arch08_pump_vdot</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>Arch08_pump_delta_p</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>Arch08_radiator_vdot</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>Arch08_perc_recirc</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>Arch08_radiator_t_in</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>Arch08_pump2_vdot</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>Arch08_pump2_delta_p</t>
         </is>
       </c>
     </row>
@@ -495,37 +685,151 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1666666666666667</v>
+        <v>4.450185481690071</v>
       </c>
       <c r="C2" t="n">
-        <v>0.03078718242887758</v>
+        <v>0.8514626862125846</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1358798175711224</v>
+        <v>2.801789788181221</v>
       </c>
       <c r="E2" t="n">
-        <v>306.6674606968199</v>
+        <v>0.4069926429198999</v>
       </c>
       <c r="F2" t="n">
-        <v>315.1035309651432</v>
+        <v>350.4658620008473</v>
       </c>
       <c r="G2" t="n">
-        <v>310.9716196524392</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>307.6614797046352</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>320.3861989161594</v>
+        <v>2.888123329426568</v>
       </c>
       <c r="J2" t="n">
-        <v>306.6674606968199</v>
+        <v>0.8626512437973369</v>
       </c>
       <c r="K2" t="n">
-        <v>325.6796778876807</v>
+        <v>2.888123329426568</v>
       </c>
       <c r="L2" t="n">
-        <v>0.07606633230618498</v>
+        <v>0.3856766953822806</v>
+      </c>
+      <c r="M2" t="n">
+        <v>350.0960212196717</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1.562062152263526</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.4883594712484415</v>
+      </c>
+      <c r="P2" t="n">
+        <v>2.801789788181182</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.8514626862125805</v>
+      </c>
+      <c r="R2" t="n">
+        <v>2.801789788181182</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.4069926429199102</v>
+      </c>
+      <c r="T2" t="n">
+        <v>350.4658620008472</v>
+      </c>
+      <c r="U2" t="n">
+        <v>1.648395693508894</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.4883594712484383</v>
+      </c>
+      <c r="W2" t="n">
+        <v>4.050185481690083</v>
+      </c>
+      <c r="X2" t="n">
+        <v>1.078659216789787</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>2.655048059122277</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.3444626002623554</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>351.15</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>1.150137654383575</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0.3951064726207478</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>1.150137654383575</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.8033303458047129</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>348.5376798925576</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>4.050207553797597</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0.488363955115131</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>4.450734703437816</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0.6155671974011956</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.9815442324479584</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.8511685214798289</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>348.0525533136284</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>4.450185481690091</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0.8514626862125869</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>2.801789788181203</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>0.4069926429199072</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>350.4658620008472</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -533,303 +837,151 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2</v>
+        <v>3.642970144500962</v>
       </c>
       <c r="C3" t="n">
-        <v>0.03719881950877927</v>
+        <v>0.658593489588416</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1628011804912188</v>
+        <v>2.476392880716794</v>
       </c>
       <c r="E3" t="n">
-        <v>309.4205584734395</v>
+        <v>0.3597249471328955</v>
       </c>
       <c r="F3" t="n">
-        <v>316.3973690341517</v>
+        <v>352.0930985208799</v>
       </c>
       <c r="G3" t="n">
-        <v>312.9793391096121</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>310.2422489515129</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>320.7688472191118</v>
+        <v>2.558119529921713</v>
       </c>
       <c r="J3" t="n">
-        <v>309.4205584734395</v>
+        <v>0.669185008338227</v>
       </c>
       <c r="K3" t="n">
-        <v>325.2580534501679</v>
+        <v>2.558119529921713</v>
       </c>
       <c r="L3" t="n">
-        <v>0.1014861590692906</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.04684844280810583</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.2031515571918942</v>
-      </c>
-      <c r="E4" t="n">
-        <v>312.1704476099254</v>
-      </c>
-      <c r="F4" t="n">
-        <v>317.70676633787</v>
-      </c>
-      <c r="G4" t="n">
-        <v>314.9938973253738</v>
-      </c>
-      <c r="H4" t="n">
-        <v>312.8222345175304</v>
-      </c>
-      <c r="I4" t="n">
-        <v>321.1773747330067</v>
-      </c>
-      <c r="J4" t="n">
-        <v>312.1704476099254</v>
-      </c>
-      <c r="K4" t="n">
-        <v>324.836433382633</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.1459922342955988</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.2833333333333333</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.05329556577176932</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.2300374342282307</v>
-      </c>
-      <c r="E5" t="n">
-        <v>313.4635556567899</v>
-      </c>
-      <c r="F5" t="n">
-        <v>318.3289404428087</v>
-      </c>
-      <c r="G5" t="n">
-        <v>315.9446451588739</v>
-      </c>
-      <c r="H5" t="n">
-        <v>314.036267093806</v>
-      </c>
-      <c r="I5" t="n">
-        <v>321.3795479015832</v>
-      </c>
-      <c r="J5" t="n">
-        <v>313.4635556567899</v>
-      </c>
-      <c r="K5" t="n">
-        <v>324.6380282756148</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.1799131506506343</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.3333333333333333</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.06298031427688508</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.2703526857231149</v>
-      </c>
-      <c r="E6" t="n">
-        <v>314.9177038178763</v>
-      </c>
-      <c r="F6" t="n">
-        <v>319.0339059454114</v>
-      </c>
-      <c r="G6" t="n">
-        <v>317.0165900071119</v>
-      </c>
-      <c r="H6" t="n">
-        <v>315.4021559487556</v>
-      </c>
-      <c r="I6" t="n">
-        <v>321.6152681676467</v>
-      </c>
-      <c r="J6" t="n">
-        <v>314.9177038178763</v>
-      </c>
-      <c r="K6" t="n">
-        <v>324.4148216346758</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.2371707588138338</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.3666666666666666</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.06944369957187221</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.2972233004281278</v>
-      </c>
-      <c r="E7" t="n">
-        <v>315.6665988481321</v>
-      </c>
-      <c r="F7" t="n">
-        <v>319.3992706452299</v>
-      </c>
-      <c r="G7" t="n">
-        <v>317.5698539854616</v>
-      </c>
-      <c r="H7" t="n">
-        <v>316.1058821987543</v>
-      </c>
-      <c r="I7" t="n">
-        <v>321.7403163081778</v>
-      </c>
-      <c r="J7" t="n">
-        <v>315.6665988481321</v>
-      </c>
-      <c r="K7" t="n">
-        <v>324.299834870174</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.2795938541944102</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.4166666666666667</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.07914587375499872</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.3375211262450013</v>
-      </c>
-      <c r="E8" t="n">
-        <v>316.5650743986903</v>
-      </c>
-      <c r="F8" t="n">
-        <v>319.8397726938424</v>
-      </c>
-      <c r="G8" t="n">
-        <v>318.2347508871371</v>
-      </c>
-      <c r="H8" t="n">
-        <v>316.9504326975884</v>
-      </c>
-      <c r="I8" t="n">
-        <v>321.8937813060626</v>
-      </c>
-      <c r="J8" t="n">
-        <v>316.5650743986903</v>
-      </c>
-      <c r="K8" t="n">
-        <v>324.1618541532335</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.3496029609345089</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.08561766907149518</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.3643823309285048</v>
-      </c>
-      <c r="E9" t="n">
-        <v>317.0530562460292</v>
-      </c>
-      <c r="F9" t="n">
-        <v>320.0800385932849</v>
-      </c>
-      <c r="G9" t="n">
-        <v>318.5964010967026</v>
-      </c>
-      <c r="H9" t="n">
-        <v>317.4092512500918</v>
-      </c>
-      <c r="I9" t="n">
-        <v>321.9787589386128</v>
-      </c>
-      <c r="J9" t="n">
-        <v>317.0530562460292</v>
-      </c>
-      <c r="K9" t="n">
-        <v>324.0869024983483</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0.4005256201793522</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.09532973264767332</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.4046702673523267</v>
-      </c>
-      <c r="E10" t="n">
-        <v>317.6629731430928</v>
-      </c>
-      <c r="F10" t="n">
-        <v>320.3813808876369</v>
-      </c>
-      <c r="G10" t="n">
-        <v>319.048958290813</v>
-      </c>
-      <c r="H10" t="n">
-        <v>317.9828440863042</v>
-      </c>
-      <c r="I10" t="n">
-        <v>322.0866340269861</v>
-      </c>
-      <c r="J10" t="n">
-        <v>317.6629731430928</v>
-      </c>
-      <c r="K10" t="n">
-        <v>323.9932120428593</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0.4832860087924997</v>
+        <v>0.33452377488544</v>
+      </c>
+      <c r="M3" t="n">
+        <v>351.6452198557627</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1.084850614579245</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.3376606985933064</v>
+      </c>
+      <c r="P3" t="n">
+        <v>2.476392880716816</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.6585934895884219</v>
+      </c>
+      <c r="R3" t="n">
+        <v>2.476392880716816</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.3597249471328932</v>
+      </c>
+      <c r="T3" t="n">
+        <v>352.0930985208801</v>
+      </c>
+      <c r="U3" t="n">
+        <v>1.166577263784166</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0.3376606985933102</v>
+      </c>
+      <c r="W3" t="n">
+        <v>3.242970144500975</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0.8823237673718256</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>2.302904764207744</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0.2898779015549302</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>353.15</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>1.15022562206975</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0.3950159801028534</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>1.15022562206975</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>0.7552640287136</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>349.835675075157</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>3.242983408609135</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0.3376629564750283</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>3.643622028209654</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>0.5097909969075139</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>1.328190910382402</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>0.7089294009936845</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>348.6657143427063</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>3.642970144500978</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>0.6585934895884228</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>2.476392880716811</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>0.3597249471328939</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>352.09309852088</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>